<commit_message>
restoration and breaker fixes to match Dieters suggestions,  added MW dataviews to loadbanks as requested
</commit_message>
<xml_diff>
--- a/package/data/simtool/breakerstates/Opt5/AllBreakers_R3.xlsx
+++ b/package/data/simtool/breakerstates/Opt5/AllBreakers_R3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\12957 - Blackstart - Desktop Studies\desktopstudies\package\data\simtool\breakerstates\Opt5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozzer\Documents\TNEI\desktopstudies\package\data\simtool\breakerstates\Opt5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CBE05C-826B-46B5-9768-29A821AC6130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901839B8-72A8-4E77-B092-149E83FFE43D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="377" yWindow="377" windowWidth="24214" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allbreakers" sheetId="1" r:id="rId1"/>
@@ -1399,17 +1399,17 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E115" sqref="E115"/>
+      <selection pane="bottomRight" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.15234375" customWidth="1"/>
+    <col min="2" max="2" width="22.15234375" customWidth="1"/>
+    <col min="25" max="25" width="9.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="108" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
@@ -1524,7 +1524,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -1641,7 +1641,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>129</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>129</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>129</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>129</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>129</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>129</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>129</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>129</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>129</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>129</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>129</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>129</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>129</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>129</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>129</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>129</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>129</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>129</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>129</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>129</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>129</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>129</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>129</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>129</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>129</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>129</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
         <v>129</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>129</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>129</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>129</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>129</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>129</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="s">
         <v>129</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>129</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
         <v>129</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>129</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
         <v>129</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>129</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>129</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
         <v>129</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>129</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>129</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>129</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A49" s="5" t="s">
         <v>129</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A50" s="5" t="s">
         <v>129</v>
       </c>
@@ -7353,7 +7353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>129</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>129</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>129</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
         <v>129</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>129</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>129</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
         <v>129</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">
         <v>129</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>129</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>129</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>130</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>130</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>130</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>130</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>130</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
         <v>130</v>
       </c>
@@ -9257,7 +9257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
         <v>130</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>130</v>
       </c>
@@ -9495,7 +9495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
         <v>130</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A70" s="5" t="s">
         <v>130</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A71" s="5" t="s">
         <v>130</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A72" s="5" t="s">
         <v>131</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>131</v>
       </c>
@@ -10090,7 +10090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A74" s="5" t="s">
         <v>132</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A75" s="5" t="s">
         <v>132</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A76" s="5" t="s">
         <v>132</v>
       </c>
@@ -10447,7 +10447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A77" s="5" t="s">
         <v>132</v>
       </c>
@@ -10566,7 +10566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A78" s="5" t="s">
         <v>132</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A79" s="5" t="s">
         <v>132</v>
       </c>
@@ -10804,7 +10804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A80" s="5" t="s">
         <v>136</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A81" s="5" t="s">
         <v>136</v>
       </c>
@@ -11042,7 +11042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A82" s="5" t="s">
         <v>136</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A83" s="5" t="s">
         <v>134</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A84" s="5" t="s">
         <v>134</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A85" s="5" t="s">
         <v>134</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A86" s="5" t="s">
         <v>134</v>
       </c>
@@ -11637,7 +11637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A87" s="5" t="s">
         <v>134</v>
       </c>
@@ -11756,7 +11756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A88" s="5" t="s">
         <v>134</v>
       </c>
@@ -11875,7 +11875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A89" s="5" t="s">
         <v>134</v>
       </c>
@@ -11994,7 +11994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A90" s="5" t="s">
         <v>133</v>
       </c>
@@ -12113,7 +12113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A91" s="5" t="s">
         <v>133</v>
       </c>
@@ -12232,7 +12232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A92" s="5" t="s">
         <v>133</v>
       </c>
@@ -12351,7 +12351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A93" s="5" t="s">
         <v>133</v>
       </c>
@@ -12470,7 +12470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A94" s="5" t="s">
         <v>133</v>
       </c>
@@ -12589,7 +12589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>133</v>
       </c>
@@ -12708,7 +12708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A96" s="5" t="s">
         <v>133</v>
       </c>
@@ -12827,7 +12827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A97" s="5" t="s">
         <v>135</v>
       </c>
@@ -12946,7 +12946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A98" s="5" t="s">
         <v>137</v>
       </c>
@@ -13065,7 +13065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>137</v>
       </c>
@@ -13073,7 +13073,7 @@
         <v>109</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
         <v>3</v>
@@ -13184,7 +13184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A100" s="5" t="s">
         <v>137</v>
       </c>
@@ -13303,7 +13303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
         <v>137</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>137</v>
       </c>
@@ -13541,7 +13541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
         <v>137</v>
       </c>
@@ -13660,7 +13660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
         <v>137</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A105" s="5" t="s">
         <v>137</v>
       </c>
@@ -13898,7 +13898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>137</v>
       </c>
@@ -14017,7 +14017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A107" s="5" t="s">
         <v>137</v>
       </c>
@@ -14136,7 +14136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>137</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A109" s="5" t="s">
         <v>137</v>
       </c>
@@ -14374,7 +14374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A110" s="5" t="s">
         <v>137</v>
       </c>
@@ -14493,7 +14493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A111" s="5" t="s">
         <v>137</v>
       </c>
@@ -14612,7 +14612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A112" s="5" t="s">
         <v>137</v>
       </c>
@@ -14731,7 +14731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A113" s="5" t="s">
         <v>137</v>
       </c>
@@ -14850,7 +14850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A114" s="5" t="s">
         <v>137</v>
       </c>
@@ -14969,7 +14969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A115" s="5" t="s">
         <v>137</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A116" s="5" t="s">
         <v>137</v>
       </c>
@@ -15207,7 +15207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A117" s="5" t="s">
         <v>137</v>
       </c>
@@ -15326,7 +15326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A118" s="5" t="s">
         <v>137</v>
       </c>
@@ -15445,7 +15445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A119" s="5" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
Stevens croft steps logic fix
</commit_message>
<xml_diff>
--- a/package/data/simtool/breakerstates/Opt5/AllBreakers_R3.xlsx
+++ b/package/data/simtool/breakerstates/Opt5/AllBreakers_R3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\National Grid\12957 - Black Start NIC\6 - OS&amp;T WS\Desktop exercises\Lookup tables\Revision 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozzer\Documents\TNEI\desktopstudies\package\data\simtool\breakerstates\Opt5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63256AF-A463-43E8-A9BE-4C8DD2126629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC734AD-B95A-4587-876E-0A8E9528DED0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="377" yWindow="377" windowWidth="24214" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allbreakers" sheetId="1" r:id="rId1"/>
@@ -1396,21 +1396,21 @@
   <dimension ref="A1:AM119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D101" sqref="D101"/>
+      <selection pane="bottomRight" activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.15234375" customWidth="1"/>
+    <col min="2" max="2" width="22.15234375" customWidth="1"/>
+    <col min="4" max="4" width="10.3828125" customWidth="1"/>
+    <col min="25" max="25" width="9.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="108" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
@@ -1525,7 +1525,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>128</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>128</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>128</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>128</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>128</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>128</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>128</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>128</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>128</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>128</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>128</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>128</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>128</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>128</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>128</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>128</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>128</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>128</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>128</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>128</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>128</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>128</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>128</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>128</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>128</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>128</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>128</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
         <v>128</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>128</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>128</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>128</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>128</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>128</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="s">
         <v>128</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>128</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
         <v>128</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>128</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
         <v>128</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>128</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>128</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
         <v>128</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>128</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
         <v>128</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>128</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A49" s="5" t="s">
         <v>128</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A50" s="5" t="s">
         <v>128</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>128</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>128</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>128</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
         <v>128</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>128</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>128</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
         <v>128</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">
         <v>128</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>128</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>128</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>129</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>129</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>129</v>
       </c>
@@ -8901,7 +8901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>129</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>129</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
         <v>129</v>
       </c>
@@ -9258,7 +9258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
         <v>129</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>129</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
         <v>129</v>
       </c>
@@ -9615,7 +9615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A70" s="5" t="s">
         <v>129</v>
       </c>
@@ -9734,7 +9734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A71" s="5" t="s">
         <v>129</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A72" s="5" t="s">
         <v>130</v>
       </c>
@@ -9972,7 +9972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>130</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A74" s="5" t="s">
         <v>131</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A75" s="5" t="s">
         <v>131</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A76" s="5" t="s">
         <v>131</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A77" s="5" t="s">
         <v>131</v>
       </c>
@@ -10567,7 +10567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A78" s="5" t="s">
         <v>131</v>
       </c>
@@ -10686,7 +10686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A79" s="5" t="s">
         <v>131</v>
       </c>
@@ -10805,7 +10805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A80" s="5" t="s">
         <v>135</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A81" s="5" t="s">
         <v>135</v>
       </c>
@@ -11043,7 +11043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A82" s="5" t="s">
         <v>135</v>
       </c>
@@ -11162,7 +11162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A83" s="5" t="s">
         <v>133</v>
       </c>
@@ -11281,7 +11281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A84" s="5" t="s">
         <v>133</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A85" s="5" t="s">
         <v>133</v>
       </c>
@@ -11519,7 +11519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A86" s="5" t="s">
         <v>133</v>
       </c>
@@ -11638,7 +11638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A87" s="5" t="s">
         <v>133</v>
       </c>
@@ -11757,7 +11757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A88" s="5" t="s">
         <v>133</v>
       </c>
@@ -11876,7 +11876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A89" s="5" t="s">
         <v>133</v>
       </c>
@@ -11995,7 +11995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A90" s="5" t="s">
         <v>132</v>
       </c>
@@ -12114,7 +12114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A91" s="5" t="s">
         <v>132</v>
       </c>
@@ -12233,7 +12233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A92" s="5" t="s">
         <v>132</v>
       </c>
@@ -12352,7 +12352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A93" s="5" t="s">
         <v>132</v>
       </c>
@@ -12471,7 +12471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A94" s="5" t="s">
         <v>132</v>
       </c>
@@ -12590,7 +12590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>132</v>
       </c>
@@ -12709,7 +12709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A96" s="5" t="s">
         <v>132</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A97" s="5" t="s">
         <v>134</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A98" s="5" t="s">
         <v>136</v>
       </c>
@@ -13066,7 +13066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>136</v>
       </c>
@@ -13185,7 +13185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A100" s="5" t="s">
         <v>136</v>
       </c>
@@ -13304,7 +13304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
         <v>136</v>
       </c>
@@ -13423,7 +13423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>136</v>
       </c>
@@ -13542,7 +13542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
         <v>136</v>
       </c>
@@ -13661,7 +13661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
         <v>136</v>
       </c>
@@ -13780,7 +13780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A105" s="5" t="s">
         <v>136</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>136</v>
       </c>
@@ -14018,7 +14018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A107" s="5" t="s">
         <v>136</v>
       </c>
@@ -14137,7 +14137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>136</v>
       </c>
@@ -14256,7 +14256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A109" s="5" t="s">
         <v>136</v>
       </c>
@@ -14375,7 +14375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A110" s="5" t="s">
         <v>136</v>
       </c>
@@ -14494,7 +14494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A111" s="5" t="s">
         <v>136</v>
       </c>
@@ -14613,7 +14613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A112" s="5" t="s">
         <v>136</v>
       </c>
@@ -14732,7 +14732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A113" s="5" t="s">
         <v>136</v>
       </c>
@@ -14851,7 +14851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A114" s="5" t="s">
         <v>136</v>
       </c>
@@ -14970,7 +14970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A115" s="5" t="s">
         <v>136</v>
       </c>
@@ -15089,7 +15089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A116" s="5" t="s">
         <v>136</v>
       </c>
@@ -15103,7 +15103,7 @@
         <v>3</v>
       </c>
       <c r="E116" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F116" t="s">
         <v>1</v>
@@ -15208,7 +15208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A117" s="5" t="s">
         <v>136</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A118" s="5" t="s">
         <v>136</v>
       </c>
@@ -15446,7 +15446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A119" s="5" t="s">
         <v>136</v>
       </c>

</xml_diff>